<commit_message>
All ready for conductiong experimants: root@poweredge320:~/tools/DockerNET# ./ipt 7     — with iptables root@poweredge320:~/tools/DockerNET# ./ipipe 3    — with pipework
</commit_message>
<xml_diff>
--- a/iperf.xlsx
+++ b/iperf.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="32700" windowHeight="20080" tabRatio="500"/>
+    <workbookView xWindow="12200" yWindow="2020" windowWidth="32700" windowHeight="17340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pipework" sheetId="1" r:id="rId1"/>
+    <sheet name="iptables" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>pipework</t>
   </si>
@@ -34,6 +35,10 @@
   </si>
   <si>
     <t>Pipework Inter Container Communication: N clients, 1 server (number of clients, performance Gb/s)</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Iptables Inter Container Communication: N clients, 1 server (number of clients, performance Gb/s)</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -127,8 +132,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -156,19 +163,21 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,6 +461,282 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" i="0">
+                <a:latin typeface="Helvetica Neue Medium"/>
+                <a:cs typeface="Helvetica Neue Medium"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP" b="0" i="0">
+                <a:latin typeface="Helvetica Neue Medium"/>
+                <a:cs typeface="Helvetica Neue Medium"/>
+              </a:rPr>
+              <a:t>Iptables ICC: N clients, 1 server (number of clients, performance Gb/s)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>iptables!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>iptables!$B$12:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.984999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.883333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.172499999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.428</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.921666666666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.021428571428571</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.11625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>iptables!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>iptables!$B$13:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>iptables!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StDev</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>iptables!$B$14:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53033008588991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.476060220280306</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.378186461947014</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.343831354009491</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7193168054944</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.482611941122768</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.405213788370676</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:axId val="-2109019144"/>
+        <c:axId val="-2107752728"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2109019144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2107752728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2107752728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="dot"/>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="#\ ##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2109019144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0">
+              <a:latin typeface="Helvetica Neue Light"/>
+              <a:cs typeface="Helvetica Neue Light"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup paperSize="9" orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -471,6 +756,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -811,7 +1133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -1173,4 +1495,372 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>6</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3">
+        <v>3.22</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3">
+        <v>3.73</v>
+      </c>
+      <c r="H6" s="3">
+        <v>4</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3">
+        <v>3.73</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3.44</v>
+      </c>
+      <c r="H7" s="3">
+        <v>2.71</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3.33</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2.63</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3">
+        <v>5.34</v>
+      </c>
+      <c r="E9" s="3">
+        <v>4.57</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3.75</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2.37</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2.64</v>
+      </c>
+      <c r="I9" s="3">
+        <v>3.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3">
+        <v>8.36</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3.42</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2.99</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="C11" s="3">
+        <v>7.61</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4.92</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2.91</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2.48</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2.96</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5">
+        <f>AVERAGE(B4:B11)</f>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" ref="C12:I12" si="0">AVERAGE(C4:C11)</f>
+        <v>7.9849999999999994</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>4.8833333333333337</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>4.1724999999999994</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>3.4279999999999999</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
+        <v>2.9216666666666664</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="0"/>
+        <v>3.0214285714285714</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="0"/>
+        <v>2.11625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5">
+        <f>SUM(B4:B11)</f>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" ref="C13:I13" si="1">SUM(C4:C11)</f>
+        <v>15.969999999999999</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="1"/>
+        <v>14.65</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>16.689999999999998</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="1"/>
+        <v>17.14</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="1"/>
+        <v>17.529999999999998</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="1"/>
+        <v>21.15</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="1"/>
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5">
+        <f>_xlfn.STDEV.P(B4:B11)</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <f>STDEVA(C4:C11)</f>
+        <v>0.53033008588991004</v>
+      </c>
+      <c r="D14" s="5">
+        <f>STDEVA(D4:D11)</f>
+        <v>0.47606022028030598</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" ref="E14:I14" si="2">STDEVA(E4:E11)</f>
+        <v>0.37818646194701377</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="2"/>
+        <v>0.34383135400949105</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="2"/>
+        <v>0.71931680549439958</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="2"/>
+        <v>0.48261194112276767</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" si="2"/>
+        <v>0.40521378837067568</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <phoneticPr fontId="5"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created multiserver version for pipeworks and ovs.
</commit_message>
<xml_diff>
--- a/iperf.xlsx
+++ b/iperf.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12200" yWindow="2020" windowWidth="32700" windowHeight="17340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9580" yWindow="2020" windowWidth="40980" windowHeight="20900" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pipework" sheetId="1" r:id="rId1"/>
-    <sheet name="iptables" sheetId="2" r:id="rId2"/>
+    <sheet name="pipework multiserver" sheetId="3" r:id="rId2"/>
+    <sheet name="iptables" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>pipework</t>
   </si>
@@ -34,11 +35,23 @@
     <t>StDev</t>
   </si>
   <si>
-    <t>Pipework Inter Container Communication: N clients, 1 server (number of clients, performance Gb/s)</t>
+    <t>Iptables Inter Container Communication: N clients, 1 server (number of clients, performance Gb/s)</t>
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>Iptables Inter Container Communication: N clients, 1 server (number of clients, performance Gb/s)</t>
+    <t>clients</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>servers</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Pipework Inter Container Communication: N clients, M servers (performance Gb/s)</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Pipework Inter Container Communication: N clients, 1 server (performance Gb/s)</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -47,7 +60,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="#\ ##0.0"/>
+    <numFmt numFmtId="176" formatCode="#\ ##0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -109,7 +122,7 @@
       <name val="Helvetica Neue Medium"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,8 +135,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -131,8 +150,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -148,22 +196,66 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -171,6 +263,25 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -178,6 +289,25 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -236,7 +366,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>pipework!$A$12</c:f>
+              <c:f>pipework!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -246,12 +376,60 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>pipework!$B$3:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>pipework!$B$12:$I$12</c:f>
+              <c:f>pipework!$B$24:$N$24</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>11.64</c:v>
                 </c:pt>
@@ -275,6 +453,21 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.73625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.38125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.241764705882353</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.186666666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0405</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -285,7 +478,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>pipework!$A$13</c:f>
+              <c:f>pipework!$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -295,12 +488,60 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>pipework!$B$3:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>pipework!$B$13:$I$13</c:f>
+              <c:f>pipework!$B$25:$N$25</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>11.64</c:v>
                 </c:pt>
@@ -324,6 +565,21 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>21.89</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.36</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.76</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -334,7 +590,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>pipework!$A$14</c:f>
+              <c:f>pipework!$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -344,12 +600,60 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>pipework!$B$3:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>pipework!$B$14:$I$14</c:f>
+              <c:f>pipework!$B$26:$N$26</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -373,6 +677,21 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.278205345537634</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.415898625468595</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.271505876872804</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.304823960768873</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25806975801128</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.248097497812962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -387,28 +706,29 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="-2111356504"/>
-        <c:axId val="-2113630280"/>
+        <c:axId val="2080493944"/>
+        <c:axId val="2080490872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2111356504"/>
+        <c:axId val="2080493944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113630280"/>
+        <c:crossAx val="2080490872"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
+        <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113630280"/>
+        <c:axId val="2080490872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +746,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111356504"/>
+        <c:crossAx val="2080493944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -492,6 +812,598 @@
                 <a:latin typeface="Helvetica Neue Medium"/>
                 <a:cs typeface="Helvetica Neue Medium"/>
               </a:rPr>
+              <a:t>Pipework ICC: N clients, M servers (performance Gb/s)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pipework multiserver'!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'pipework multiserver'!$B$2:$N$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="13"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>12</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>20</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>20</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'pipework multiserver'!$B$24:$N$24</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>9.985</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.356666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5075</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9525</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.075833333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.475625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.082</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.575333333333333</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.194</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.398333333333333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2545</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pipework multiserver'!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'pipework multiserver'!$B$2:$N$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="13"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>12</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>20</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>20</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'pipework multiserver'!$B$25:$N$25</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>19.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.07</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.91</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.61</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.63</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23.88</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.39</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pipework multiserver'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StDev</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'pipework multiserver'!$B$2:$N$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="13"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>12</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>20</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>20</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'pipework multiserver'!$B$26:$N$26</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.0636396103067892</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.313515018247399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0757187779440039</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.297139136881473</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.348045563519654</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.261480342850032</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.221929981450606</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.599349647534726</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.288020061029705</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.285328549136569</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.333630744512867</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.541679487027766</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.444350205652206</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:axId val="2128012712"/>
+        <c:axId val="2129757048"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2128012712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2129757048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2129757048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="dot"/>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="#\ ##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2128012712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0">
+              <a:latin typeface="Helvetica Neue Light"/>
+              <a:cs typeface="Helvetica Neue Light"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup paperSize="9" orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" i="0">
+                <a:latin typeface="Helvetica Neue Medium"/>
+                <a:cs typeface="Helvetica Neue Medium"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP" b="0" i="0">
+                <a:latin typeface="Helvetica Neue Medium"/>
+                <a:cs typeface="Helvetica Neue Medium"/>
+              </a:rPr>
               <a:t>Iptables ICC: N clients, 1 server (number of clients, performance Gb/s)</a:t>
             </a:r>
           </a:p>
@@ -663,11 +1575,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="-2109019144"/>
-        <c:axId val="-2107752728"/>
+        <c:axId val="2080442904"/>
+        <c:axId val="2080439832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2109019144"/>
+        <c:axId val="2080442904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,7 +1588,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107752728"/>
+        <c:crossAx val="2080439832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -684,7 +1596,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2107752728"/>
+        <c:axId val="2080439832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -702,7 +1614,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109019144"/>
+        <c:crossAx val="2080442904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -741,16 +1653,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -773,6 +1685,43 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1131,10 +2080,1744 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>6</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4">
+        <v>8</v>
+      </c>
+      <c r="J3" s="4">
+        <v>16</v>
+      </c>
+      <c r="K3" s="4">
+        <v>17</v>
+      </c>
+      <c r="L3" s="4">
+        <v>18</v>
+      </c>
+      <c r="M3" s="4">
+        <v>19</v>
+      </c>
+      <c r="N3" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>11.64</v>
+      </c>
+      <c r="C4" s="3">
+        <v>8.06</v>
+      </c>
+      <c r="D4" s="3">
+        <v>6.77</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5.59</v>
+      </c>
+      <c r="F4" s="3">
+        <v>4.71</v>
+      </c>
+      <c r="G4" s="3">
+        <v>4.09</v>
+      </c>
+      <c r="H4" s="3">
+        <v>3.69</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2.89</v>
+      </c>
+      <c r="J4">
+        <v>2.23</v>
+      </c>
+      <c r="K4">
+        <v>1.56</v>
+      </c>
+      <c r="L4">
+        <v>1.43</v>
+      </c>
+      <c r="M4">
+        <v>1.59</v>
+      </c>
+      <c r="N4">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6.76</v>
+      </c>
+      <c r="E5" s="3">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3.64</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2.94</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="J5">
+        <v>1.79</v>
+      </c>
+      <c r="K5">
+        <v>1.87</v>
+      </c>
+      <c r="L5">
+        <v>1.57</v>
+      </c>
+      <c r="M5">
+        <v>1.24</v>
+      </c>
+      <c r="N5">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3">
+        <v>5.67</v>
+      </c>
+      <c r="E6" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3.74</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3.41</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2.87</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="J6">
+        <v>1.66</v>
+      </c>
+      <c r="K6">
+        <v>1.55</v>
+      </c>
+      <c r="L6">
+        <v>1.52</v>
+      </c>
+      <c r="M6">
+        <v>1.2</v>
+      </c>
+      <c r="N6">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3">
+        <v>5.21</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3.33</v>
+      </c>
+      <c r="H7" s="3">
+        <v>2.73</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="J7">
+        <v>1.22</v>
+      </c>
+      <c r="K7">
+        <v>1.3</v>
+      </c>
+      <c r="L7">
+        <v>1.73</v>
+      </c>
+      <c r="M7">
+        <v>1.43</v>
+      </c>
+      <c r="N7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="F8" s="3">
+        <v>3.92</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3.41</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3.09</v>
+      </c>
+      <c r="I8" s="3">
+        <v>2.74</v>
+      </c>
+      <c r="J8">
+        <v>1.96</v>
+      </c>
+      <c r="K8">
+        <v>1.33</v>
+      </c>
+      <c r="L8">
+        <v>1.68</v>
+      </c>
+      <c r="M8">
+        <v>0.85</v>
+      </c>
+      <c r="N8">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="G9" s="3">
+        <v>3.65</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3.12</v>
+      </c>
+      <c r="I9" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J9">
+        <v>1.18</v>
+      </c>
+      <c r="K9">
+        <v>1.22</v>
+      </c>
+      <c r="L9">
+        <v>1.29</v>
+      </c>
+      <c r="M9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N9">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="H10" s="3">
+        <v>3.72</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2.31</v>
+      </c>
+      <c r="J10">
+        <v>1.89</v>
+      </c>
+      <c r="K10">
+        <v>0.89</v>
+      </c>
+      <c r="L10">
+        <v>0.98</v>
+      </c>
+      <c r="M10">
+        <v>1.24</v>
+      </c>
+      <c r="N10">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="J11">
+        <v>0.9</v>
+      </c>
+      <c r="K11">
+        <v>0.8</v>
+      </c>
+      <c r="L11">
+        <v>0.82</v>
+      </c>
+      <c r="M11">
+        <v>1.23</v>
+      </c>
+      <c r="N11">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="K12">
+        <v>1.23</v>
+      </c>
+      <c r="L12">
+        <v>0.94</v>
+      </c>
+      <c r="M12">
+        <v>0.86</v>
+      </c>
+      <c r="N12">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13">
+        <v>0.9</v>
+      </c>
+      <c r="K13">
+        <v>1.06</v>
+      </c>
+      <c r="L13">
+        <v>0.91</v>
+      </c>
+      <c r="M13">
+        <v>0.92</v>
+      </c>
+      <c r="N13">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="1">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14">
+        <v>0.96</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1.02</v>
+      </c>
+      <c r="M14">
+        <v>0.83</v>
+      </c>
+      <c r="N14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15">
+        <v>1.22</v>
+      </c>
+      <c r="K15">
+        <v>1.21</v>
+      </c>
+      <c r="L15">
+        <v>0.98</v>
+      </c>
+      <c r="M15">
+        <v>0.85</v>
+      </c>
+      <c r="N15">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="1">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16">
+        <v>1.19</v>
+      </c>
+      <c r="K16">
+        <v>0.93</v>
+      </c>
+      <c r="L16">
+        <v>1.06</v>
+      </c>
+      <c r="M16">
+        <v>0.8</v>
+      </c>
+      <c r="N16">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17">
+        <v>0.93</v>
+      </c>
+      <c r="K17">
+        <v>1.08</v>
+      </c>
+      <c r="L17">
+        <v>1.31</v>
+      </c>
+      <c r="M17">
+        <v>0.94</v>
+      </c>
+      <c r="N17">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="1">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18">
+        <v>1.42</v>
+      </c>
+      <c r="K18">
+        <v>1.36</v>
+      </c>
+      <c r="L18">
+        <v>0.78</v>
+      </c>
+      <c r="M18">
+        <v>0.69</v>
+      </c>
+      <c r="N18">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="1">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19">
+        <v>1.49</v>
+      </c>
+      <c r="K19">
+        <v>1.36</v>
+      </c>
+      <c r="L19">
+        <v>0.99</v>
+      </c>
+      <c r="M19">
+        <v>0.75</v>
+      </c>
+      <c r="N19">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="1">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20">
+        <v>1.36</v>
+      </c>
+      <c r="L20">
+        <v>0.96</v>
+      </c>
+      <c r="M20">
+        <v>0.96</v>
+      </c>
+      <c r="N20">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="L21">
+        <v>1.39</v>
+      </c>
+      <c r="M21">
+        <v>0.88</v>
+      </c>
+      <c r="N21">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="1">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="M22">
+        <v>1.4</v>
+      </c>
+      <c r="N22">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="N23">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5">
+        <f>AVERAGE(B4:B23)</f>
+        <v>11.64</v>
+      </c>
+      <c r="C24" s="5">
+        <f>AVERAGE(C4:C9)</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D24" s="5">
+        <f>AVERAGE(D4:D8)</f>
+        <v>6.3999999999999995</v>
+      </c>
+      <c r="E24" s="5">
+        <f>AVERAGE(E4:E7)</f>
+        <v>5.1475</v>
+      </c>
+      <c r="F24" s="5">
+        <f>AVERAGE(F4:F8)</f>
+        <v>4.3</v>
+      </c>
+      <c r="G24" s="5">
+        <f>AVERAGE(G4:G9)</f>
+        <v>3.5883333333333334</v>
+      </c>
+      <c r="H24" s="5">
+        <f>AVERAGE(H4:H10)</f>
+        <v>3.1657142857142859</v>
+      </c>
+      <c r="I24" s="5">
+        <f>AVERAGE(I4:I23)</f>
+        <v>2.7362499999999996</v>
+      </c>
+      <c r="J24" s="5">
+        <f>AVERAGE(J4:J23)</f>
+        <v>1.3812499999999999</v>
+      </c>
+      <c r="K24" s="5">
+        <f>AVERAGE(K4:K23)</f>
+        <v>1.2417647058823529</v>
+      </c>
+      <c r="L24" s="5">
+        <f>AVERAGE(L4:L23)</f>
+        <v>1.1866666666666665</v>
+      </c>
+      <c r="M24" s="5">
+        <f>AVERAGE(M4:M23)</f>
+        <v>1.0399999999999998</v>
+      </c>
+      <c r="N24" s="5">
+        <f>AVERAGE(N4:N23)</f>
+        <v>1.0405000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="5">
+        <f>SUM(B4:B10)</f>
+        <v>11.64</v>
+      </c>
+      <c r="C25" s="5">
+        <f>SUM(C4:C9)</f>
+        <v>16.600000000000001</v>
+      </c>
+      <c r="D25" s="5">
+        <f>SUM(D4:D8)</f>
+        <v>19.2</v>
+      </c>
+      <c r="E25" s="5">
+        <f>SUM(E4:E7)</f>
+        <v>20.59</v>
+      </c>
+      <c r="F25" s="5">
+        <f>SUM(F4:F8)</f>
+        <v>21.5</v>
+      </c>
+      <c r="G25" s="5">
+        <f>SUM(G4:G9)</f>
+        <v>21.53</v>
+      </c>
+      <c r="H25" s="5">
+        <f>SUM(H4:H10)</f>
+        <v>22.16</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" ref="C25:J25" si="0">SUM(I4:I11)</f>
+        <v>21.889999999999997</v>
+      </c>
+      <c r="J25" s="5">
+        <f>SUM(J4:J23)</f>
+        <v>22.099999999999998</v>
+      </c>
+      <c r="K25" s="5">
+        <f>SUM(K4:K23)</f>
+        <v>21.11</v>
+      </c>
+      <c r="L25" s="5">
+        <f>SUM(L4:L23)</f>
+        <v>21.36</v>
+      </c>
+      <c r="M25" s="5">
+        <f>SUM(M4:M23)</f>
+        <v>19.759999999999998</v>
+      </c>
+      <c r="N25" s="5">
+        <f>SUM(N4:N23)</f>
+        <v>20.810000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="5">
+        <f>_xlfn.STDEV.P(B4:B10)</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="5">
+        <f>STDEVA(C4:C9)</f>
+        <v>0.33941125496954189</v>
+      </c>
+      <c r="D26" s="5">
+        <f>STDEVA(D4:D8)</f>
+        <v>0.63221831672294959</v>
+      </c>
+      <c r="E26" s="5">
+        <f>STDEVA(E4:E7)</f>
+        <v>0.33029027637317243</v>
+      </c>
+      <c r="F26" s="5">
+        <f>STDEVA(F4:F8)</f>
+        <v>0.44659825346725224</v>
+      </c>
+      <c r="G26" s="5">
+        <f>STDEVA(G4:G9)</f>
+        <v>0.27874121809783819</v>
+      </c>
+      <c r="H26" s="5">
+        <f>STDEVA(H4:H10)</f>
+        <v>0.39118866474959507</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" ref="E26:J26" si="1">STDEVA(I4:I11)</f>
+        <v>0.27820534553763399</v>
+      </c>
+      <c r="J26" s="5">
+        <f>STDEVA(J4:J23)</f>
+        <v>0.41589862546859518</v>
+      </c>
+      <c r="K26" s="5">
+        <f>STDEVA(K4:K23)</f>
+        <v>0.27150587687280403</v>
+      </c>
+      <c r="L26" s="5">
+        <f>STDEVA(L4:L23)</f>
+        <v>0.30482396076887308</v>
+      </c>
+      <c r="M26" s="5">
+        <f>STDEVA(M4:M23)</f>
+        <v>0.25806975801127979</v>
+      </c>
+      <c r="N26" s="5">
+        <f>STDEVA(N4:N23)</f>
+        <v>0.24809749781296203</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N1"/>
+  </mergeCells>
+  <phoneticPr fontId="5"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="12">
+        <v>2</v>
+      </c>
+      <c r="C2" s="12">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12">
+        <v>3</v>
+      </c>
+      <c r="E2" s="12">
+        <v>4</v>
+      </c>
+      <c r="F2" s="12">
+        <v>4</v>
+      </c>
+      <c r="G2" s="12">
+        <v>4</v>
+      </c>
+      <c r="H2" s="12">
+        <v>4</v>
+      </c>
+      <c r="I2" s="12">
+        <v>5</v>
+      </c>
+      <c r="J2" s="12">
+        <v>5</v>
+      </c>
+      <c r="K2" s="12">
+        <v>5</v>
+      </c>
+      <c r="L2" s="12">
+        <v>5</v>
+      </c>
+      <c r="M2" s="12">
+        <v>6</v>
+      </c>
+      <c r="N2" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9">
+        <v>4</v>
+      </c>
+      <c r="F3" s="9">
+        <v>8</v>
+      </c>
+      <c r="G3" s="9">
+        <v>12</v>
+      </c>
+      <c r="H3" s="9">
+        <v>16</v>
+      </c>
+      <c r="I3" s="9">
+        <v>5</v>
+      </c>
+      <c r="J3" s="9">
+        <v>10</v>
+      </c>
+      <c r="K3" s="9">
+        <v>15</v>
+      </c>
+      <c r="L3" s="9">
+        <v>20</v>
+      </c>
+      <c r="M3" s="9">
+        <v>6</v>
+      </c>
+      <c r="N3" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>10.029999999999999</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5.68</v>
+      </c>
+      <c r="D4" s="3">
+        <v>7.41</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3.27</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2.63</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1.36</v>
+      </c>
+      <c r="I4" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J4">
+        <v>2.83</v>
+      </c>
+      <c r="K4">
+        <v>2.17</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>3.76</v>
+      </c>
+      <c r="N4">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>9.94</v>
+      </c>
+      <c r="C5" s="2">
+        <v>6.07</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7.39</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5.19</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2.85</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3.68</v>
+      </c>
+      <c r="J5">
+        <v>2.31</v>
+      </c>
+      <c r="K5">
+        <v>1.73</v>
+      </c>
+      <c r="L5">
+        <v>1.87</v>
+      </c>
+      <c r="M5">
+        <v>3.88</v>
+      </c>
+      <c r="N5">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5.36</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7.27</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5.53</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3.44</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3.73</v>
+      </c>
+      <c r="J6">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="K6">
+        <v>1.97</v>
+      </c>
+      <c r="L6">
+        <v>1.25</v>
+      </c>
+      <c r="M6">
+        <v>3.62</v>
+      </c>
+      <c r="N6">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2">
+        <v>5.94</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3">
+        <v>5.41</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2.27</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2.04</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1.59</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3.56</v>
+      </c>
+      <c r="J7">
+        <v>2.44</v>
+      </c>
+      <c r="K7">
+        <v>1.96</v>
+      </c>
+      <c r="L7">
+        <v>1.33</v>
+      </c>
+      <c r="M7">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="N7">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="F8" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2.11</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1.28</v>
+      </c>
+      <c r="I8" s="3">
+        <v>4.54</v>
+      </c>
+      <c r="J8">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="K8">
+        <v>1.73</v>
+      </c>
+      <c r="L8">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="M8">
+        <v>3.65</v>
+      </c>
+      <c r="N8">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="F9">
+        <v>2.92</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1.69</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9">
+        <v>2.87</v>
+      </c>
+      <c r="K9">
+        <v>1.33</v>
+      </c>
+      <c r="L9">
+        <v>1.02</v>
+      </c>
+      <c r="M9">
+        <v>2.99</v>
+      </c>
+      <c r="N9">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="F10">
+        <v>2.91</v>
+      </c>
+      <c r="G10">
+        <v>2.21</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1.49</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10">
+        <v>2.33</v>
+      </c>
+      <c r="K10">
+        <v>1.26</v>
+      </c>
+      <c r="L10">
+        <v>0.99</v>
+      </c>
+      <c r="N10">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>2.86</v>
+      </c>
+      <c r="G11">
+        <v>1.97</v>
+      </c>
+      <c r="H11">
+        <v>1.41</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11">
+        <v>2.13</v>
+      </c>
+      <c r="K11">
+        <v>1.37</v>
+      </c>
+      <c r="L11">
+        <v>0.77</v>
+      </c>
+      <c r="N11">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3">
+        <v>2.27</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1.19</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12">
+        <v>2.1</v>
+      </c>
+      <c r="K12">
+        <v>1.49</v>
+      </c>
+      <c r="L12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N12">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1.33</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13">
+        <v>2.04</v>
+      </c>
+      <c r="K13">
+        <v>1.45</v>
+      </c>
+      <c r="L13">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="N13">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="1">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3">
+        <v>2.02</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1.39</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="K14">
+        <v>1.27</v>
+      </c>
+      <c r="L14">
+        <v>1.02</v>
+      </c>
+      <c r="N14">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3">
+        <v>1.94</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1.49</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="K15">
+        <v>1.35</v>
+      </c>
+      <c r="L15">
+        <v>0.86</v>
+      </c>
+      <c r="N15">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="1">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3">
+        <v>1.37</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="K16">
+        <v>1.33</v>
+      </c>
+      <c r="L16">
+        <v>0.7</v>
+      </c>
+      <c r="N16">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3">
+        <v>1.58</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="K17">
+        <v>1.57</v>
+      </c>
+      <c r="L17">
+        <v>0.82</v>
+      </c>
+      <c r="N17">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="1">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3">
+        <v>1.21</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="K18">
+        <v>1.65</v>
+      </c>
+      <c r="L18">
+        <v>1.35</v>
+      </c>
+      <c r="N18">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="1">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3">
+        <v>1.37</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="L19">
+        <v>1.41</v>
+      </c>
+      <c r="N19">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="1">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="L20">
+        <v>1.25</v>
+      </c>
+      <c r="N20">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="L21">
+        <v>1.21</v>
+      </c>
+      <c r="N21">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="1">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="L22">
+        <v>1.17</v>
+      </c>
+      <c r="N22">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="L23">
+        <v>1.53</v>
+      </c>
+      <c r="N23">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5">
+        <f>AVERAGE(B4:B23)</f>
+        <v>9.9849999999999994</v>
+      </c>
+      <c r="C24" s="5">
+        <f>AVERAGE(C4:C23)</f>
+        <v>5.7625000000000002</v>
+      </c>
+      <c r="D24" s="5">
+        <f>AVERAGE(D4:D23)</f>
+        <v>7.3566666666666665</v>
+      </c>
+      <c r="E24" s="5">
+        <f>AVERAGE(E4:E23)</f>
+        <v>5.5075000000000003</v>
+      </c>
+      <c r="F24" s="5">
+        <f>AVERAGE(F4:F23)</f>
+        <v>2.9525000000000001</v>
+      </c>
+      <c r="G24" s="5">
+        <f>AVERAGE(G4:G23)</f>
+        <v>2.0758333333333332</v>
+      </c>
+      <c r="H24" s="5">
+        <f>AVERAGE(H4:H23)</f>
+        <v>1.4756250000000002</v>
+      </c>
+      <c r="I24" s="5">
+        <f>AVERAGE(I4:I23)</f>
+        <v>4.0819999999999999</v>
+      </c>
+      <c r="J24" s="5">
+        <f>AVERAGE(J4:J23)</f>
+        <v>2.38</v>
+      </c>
+      <c r="K24" s="5">
+        <f>AVERAGE(K4:K23)</f>
+        <v>1.5753333333333335</v>
+      </c>
+      <c r="L24" s="5">
+        <f>AVERAGE(L4:L23)</f>
+        <v>1.1940000000000002</v>
+      </c>
+      <c r="M24" s="5">
+        <f>AVERAGE(M4:M23)</f>
+        <v>3.3983333333333334</v>
+      </c>
+      <c r="N24" s="5">
+        <f>AVERAGE(N4:N23)</f>
+        <v>1.2544999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="5">
+        <f>SUM(B4:B23)</f>
+        <v>19.97</v>
+      </c>
+      <c r="C25" s="5">
+        <f>SUM(C4:C23)</f>
+        <v>23.05</v>
+      </c>
+      <c r="D25" s="5">
+        <f>SUM(D4:D23)</f>
+        <v>22.07</v>
+      </c>
+      <c r="E25" s="5">
+        <f>SUM(E4:E23)</f>
+        <v>22.03</v>
+      </c>
+      <c r="F25" s="5">
+        <f>SUM(F4:F23)</f>
+        <v>23.62</v>
+      </c>
+      <c r="G25" s="5">
+        <f>SUM(G4:G23)</f>
+        <v>24.909999999999997</v>
+      </c>
+      <c r="H25" s="5">
+        <f>SUM(H4:H23)</f>
+        <v>23.610000000000003</v>
+      </c>
+      <c r="I25" s="5">
+        <f>SUM(I4:I23)</f>
+        <v>20.41</v>
+      </c>
+      <c r="J25" s="5">
+        <f>SUM(J4:J23)</f>
+        <v>23.8</v>
+      </c>
+      <c r="K25" s="5">
+        <f>SUM(K4:K23)</f>
+        <v>23.630000000000003</v>
+      </c>
+      <c r="L25" s="5">
+        <f>SUM(L4:L23)</f>
+        <v>23.880000000000003</v>
+      </c>
+      <c r="M25" s="5">
+        <f>SUM(M4:M23)</f>
+        <v>20.39</v>
+      </c>
+      <c r="N25" s="5">
+        <f>SUM(N4:N23)</f>
+        <v>25.09</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="5">
+        <f>STDEVA(B4:B23)</f>
+        <v>6.3639610306789177E-2</v>
+      </c>
+      <c r="C26" s="5">
+        <f>STDEVA(C4:C23)</f>
+        <v>0.31351501824739864</v>
+      </c>
+      <c r="D26" s="5">
+        <f>STDEVA(D4:D23)</f>
+        <v>7.5718777944003876E-2</v>
+      </c>
+      <c r="E26" s="5">
+        <f>STDEVA(E4:E23)</f>
+        <v>0.29713913688147287</v>
+      </c>
+      <c r="F26" s="5">
+        <f>STDEVA(F4:F23)</f>
+        <v>0.34804556351965454</v>
+      </c>
+      <c r="G26" s="5">
+        <f>STDEVA(G4:G23)</f>
+        <v>0.26148034285003185</v>
+      </c>
+      <c r="H26" s="5">
+        <f>STDEVA(H4:H23)</f>
+        <v>0.22192998145060558</v>
+      </c>
+      <c r="I26" s="5">
+        <f>STDEVA(I4:I23)</f>
+        <v>0.59934964753472619</v>
+      </c>
+      <c r="J26" s="5">
+        <f>STDEVA(J4:J23)</f>
+        <v>0.28802006102970473</v>
+      </c>
+      <c r="K26" s="5">
+        <f>STDEVA(K4:K23)</f>
+        <v>0.28532854913656946</v>
+      </c>
+      <c r="L26" s="5">
+        <f>STDEVA(L4:L23)</f>
+        <v>0.33363074451286728</v>
+      </c>
+      <c r="M26" s="5">
+        <f>STDEVA(M4:M23)</f>
+        <v>0.54167948702776636</v>
+      </c>
+      <c r="N26" s="5">
+        <f>STDEVA(N4:N23)</f>
+        <v>0.44435020565220607</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N1"/>
+  </mergeCells>
+  <phoneticPr fontId="5"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1206,374 +3889,6 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="3">
-        <v>2.89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3">
-        <v>3.69</v>
-      </c>
-      <c r="I5" s="3">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3">
-        <v>4.09</v>
-      </c>
-      <c r="H6" s="3">
-        <v>2.94</v>
-      </c>
-      <c r="I6" s="3">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="1">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3">
-        <v>4.71</v>
-      </c>
-      <c r="G7" s="3">
-        <v>3.64</v>
-      </c>
-      <c r="H7" s="3">
-        <v>2.87</v>
-      </c>
-      <c r="I7" s="3">
-        <v>2.5499999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="1">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3">
-        <v>5.59</v>
-      </c>
-      <c r="F8" s="3">
-        <v>4.6900000000000004</v>
-      </c>
-      <c r="G8" s="3">
-        <v>3.41</v>
-      </c>
-      <c r="H8" s="3">
-        <v>2.73</v>
-      </c>
-      <c r="I8" s="3">
-        <v>2.74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="1">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3">
-        <v>6.77</v>
-      </c>
-      <c r="E9" s="3">
-        <v>4.8899999999999997</v>
-      </c>
-      <c r="F9" s="3">
-        <v>3.74</v>
-      </c>
-      <c r="G9" s="3">
-        <v>3.33</v>
-      </c>
-      <c r="H9" s="3">
-        <v>3.09</v>
-      </c>
-      <c r="I9" s="3">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" s="1">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3">
-        <v>8.06</v>
-      </c>
-      <c r="D10" s="3">
-        <v>6.76</v>
-      </c>
-      <c r="E10" s="3">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="F10" s="3">
-        <v>4.4400000000000004</v>
-      </c>
-      <c r="G10" s="3">
-        <v>3.41</v>
-      </c>
-      <c r="H10" s="3">
-        <v>3.12</v>
-      </c>
-      <c r="I10" s="3">
-        <v>2.31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="1">
-        <v>8</v>
-      </c>
-      <c r="B11" s="3">
-        <v>11.64</v>
-      </c>
-      <c r="C11" s="3">
-        <v>8.5399999999999991</v>
-      </c>
-      <c r="D11" s="3">
-        <v>5.67</v>
-      </c>
-      <c r="E11" s="3">
-        <v>5.21</v>
-      </c>
-      <c r="F11" s="3">
-        <v>3.92</v>
-      </c>
-      <c r="G11" s="3">
-        <v>3.65</v>
-      </c>
-      <c r="H11" s="3">
-        <v>3.72</v>
-      </c>
-      <c r="I11" s="3">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
-      <c r="A12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5">
-        <f>AVERAGE(B4:B11)</f>
-        <v>11.64</v>
-      </c>
-      <c r="C12" s="5">
-        <f t="shared" ref="C12:I12" si="0">AVERAGE(C4:C11)</f>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="D12" s="5">
-        <f t="shared" si="0"/>
-        <v>6.3999999999999995</v>
-      </c>
-      <c r="E12" s="5">
-        <f t="shared" si="0"/>
-        <v>5.1475</v>
-      </c>
-      <c r="F12" s="5">
-        <f t="shared" si="0"/>
-        <v>4.3</v>
-      </c>
-      <c r="G12" s="5">
-        <f t="shared" si="0"/>
-        <v>3.5883333333333334</v>
-      </c>
-      <c r="H12" s="5">
-        <f t="shared" si="0"/>
-        <v>3.1657142857142859</v>
-      </c>
-      <c r="I12" s="5">
-        <f t="shared" si="0"/>
-        <v>2.7362499999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
-      <c r="A13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="5">
-        <f>SUM(B4:B11)</f>
-        <v>11.64</v>
-      </c>
-      <c r="C13" s="5">
-        <f t="shared" ref="C13:I13" si="1">SUM(C4:C11)</f>
-        <v>16.600000000000001</v>
-      </c>
-      <c r="D13" s="5">
-        <f t="shared" si="1"/>
-        <v>19.2</v>
-      </c>
-      <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>20.59</v>
-      </c>
-      <c r="F13" s="5">
-        <f t="shared" si="1"/>
-        <v>21.5</v>
-      </c>
-      <c r="G13" s="5">
-        <f t="shared" si="1"/>
-        <v>21.53</v>
-      </c>
-      <c r="H13" s="5">
-        <f t="shared" si="1"/>
-        <v>22.16</v>
-      </c>
-      <c r="I13" s="5">
-        <f t="shared" si="1"/>
-        <v>21.889999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
-      <c r="A14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="5">
-        <f>_xlfn.STDEV.P(B4:B11)</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="5">
-        <f>STDEVA(C4:C11)</f>
-        <v>0.33941125496954189</v>
-      </c>
-      <c r="D14" s="5">
-        <f>STDEVA(D4:D11)</f>
-        <v>0.63221831672294959</v>
-      </c>
-      <c r="E14" s="5">
-        <f t="shared" ref="E14:I14" si="2">STDEVA(E4:E11)</f>
-        <v>0.33029027637317243</v>
-      </c>
-      <c r="F14" s="5">
-        <f t="shared" si="2"/>
-        <v>0.44659825346725224</v>
-      </c>
-      <c r="G14" s="5">
-        <f t="shared" si="2"/>
-        <v>0.27874121809783819</v>
-      </c>
-      <c r="H14" s="5">
-        <f t="shared" si="2"/>
-        <v>0.39118866474959507</v>
-      </c>
-      <c r="I14" s="5">
-        <f t="shared" si="2"/>
-        <v>0.27820534553763399</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
-  </mergeCells>
-  <phoneticPr fontId="5"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4">
-        <v>4</v>
-      </c>
-      <c r="F3" s="4">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4">
-        <v>6</v>
-      </c>
-      <c r="H3" s="4">
-        <v>7</v>
-      </c>
-      <c r="I3" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3">
         <v>1.82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Multiprocess measurements with OVS.
</commit_message>
<xml_diff>
--- a/iperf.xlsx
+++ b/iperf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="3460" windowWidth="35160" windowHeight="21880" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="6000" yWindow="5620" windowWidth="35120" windowHeight="21120" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="iptables" sheetId="2" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="pipework multiprocess" sheetId="6" r:id="rId4"/>
     <sheet name="ovs" sheetId="4" r:id="rId5"/>
     <sheet name="ovs multiserver" sheetId="5" r:id="rId6"/>
+    <sheet name="ovs multiprocess" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
   <si>
     <t>pipework</t>
   </si>
@@ -71,6 +72,10 @@
   </si>
   <si>
     <t>containers</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>OVS Inter Container Communication: N servers, M containers, L clients per container (performance Gb/s)</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -291,12 +296,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -404,7 +409,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -570,11 +574,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="2075583240"/>
-        <c:axId val="2075586296"/>
+        <c:axId val="2072891912"/>
+        <c:axId val="2042352056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2075583240"/>
+        <c:axId val="2072891912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -583,7 +587,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075586296"/>
+        <c:crossAx val="2042352056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -591,7 +595,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2075586296"/>
+        <c:axId val="2042352056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,14 +613,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075583240"/>
+        <c:crossAx val="2072891912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -680,7 +683,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1035,11 +1037,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="2074693448"/>
-        <c:axId val="2074696568"/>
+        <c:axId val="2042448248"/>
+        <c:axId val="2042451368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2074693448"/>
+        <c:axId val="2042448248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,7 +1051,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074696568"/>
+        <c:crossAx val="2042451368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1057,7 +1059,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2074696568"/>
+        <c:axId val="2042451368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,14 +1077,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074693448"/>
+        <c:crossAx val="2042448248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1146,7 +1147,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1627,11 +1627,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="2075528936"/>
-        <c:axId val="2075532056"/>
+        <c:axId val="2042508152"/>
+        <c:axId val="2042511272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2075528936"/>
+        <c:axId val="2042508152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1641,7 +1641,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075532056"/>
+        <c:crossAx val="2042511272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1649,7 +1649,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2075532056"/>
+        <c:axId val="2042511272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1667,14 +1667,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075528936"/>
+        <c:crossAx val="2042508152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2234,11 +2233,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="2098002072"/>
-        <c:axId val="2097995048"/>
+        <c:axId val="2042567560"/>
+        <c:axId val="2042570680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2098002072"/>
+        <c:axId val="2042567560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2248,7 +2247,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097995048"/>
+        <c:crossAx val="2042570680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2256,7 +2255,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097995048"/>
+        <c:axId val="2042570680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2274,7 +2273,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2098002072"/>
+        <c:crossAx val="2042567560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2700,11 +2699,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="2084825064"/>
-        <c:axId val="2084828184"/>
+        <c:axId val="2041676584"/>
+        <c:axId val="2041673048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2084825064"/>
+        <c:axId val="2041676584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2714,7 +2713,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084828184"/>
+        <c:crossAx val="2041673048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2722,7 +2721,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2084828184"/>
+        <c:axId val="2041673048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2740,7 +2739,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084825064"/>
+        <c:crossAx val="2041676584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3301,11 +3300,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="2087565320"/>
-        <c:axId val="2087568440"/>
+        <c:axId val="2041610216"/>
+        <c:axId val="2041606744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2087565320"/>
+        <c:axId val="2041610216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3315,7 +3314,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087568440"/>
+        <c:crossAx val="2041606744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3323,7 +3322,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087568440"/>
+        <c:axId val="2041606744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3341,7 +3340,614 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087565320"/>
+        <c:crossAx val="2041610216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0">
+              <a:latin typeface="Helvetica Neue Light"/>
+              <a:cs typeface="Helvetica Neue Light"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup paperSize="9" orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" i="0">
+                <a:latin typeface="Helvetica Neue Medium"/>
+                <a:cs typeface="Helvetica Neue Medium"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP" b="0" i="0">
+                <a:latin typeface="Helvetica Neue Medium"/>
+                <a:cs typeface="Helvetica Neue Medium"/>
+              </a:rPr>
+              <a:t>OVS ICC: L clients, M containers, N servers (performance Gb/s, aggregated per container)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ovs multiprocess'!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'ovs multiprocess'!$B$2:$K$4</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="10"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>16</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>16</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ovs multiprocess'!$B$25:$K$25</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>13.06</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.395</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.495</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.986874999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.058125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ovs multiprocess'!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'ovs multiprocess'!$B$2:$K$4</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="10"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>16</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>16</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ovs multiprocess'!$B$26:$K$26</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>13.06</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.79</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.78999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ovs multiprocess'!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StDev</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'ovs multiprocess'!$B$2:$K$4</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="10"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>16</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>16</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ovs multiprocess'!$B$27:$K$27</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0848528137423864</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.869741340859453</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.390768473651598</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.116761865920913</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.544985856085582</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0438510737230762</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:axId val="2084835368"/>
+        <c:axId val="2084838488"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2084835368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2084838488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2084838488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="dot"/>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="#\ ##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2084835368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3572,6 +4178,43 @@
       <xdr:col>28</xdr:col>
       <xdr:colOff>469900</xdr:colOff>
       <xdr:row>44</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3927,17 +4570,17 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
@@ -4295,22 +4938,22 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
@@ -5148,22 +5791,22 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
@@ -6022,7 +6665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -6032,19 +6675,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
@@ -6125,37 +6768,37 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>1</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>2</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <v>1</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="15">
         <v>2</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="15">
         <v>4</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="15">
         <v>1</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="15">
         <v>4</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="15">
         <v>16</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="15">
         <v>1</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="15">
         <v>16</v>
       </c>
     </row>
@@ -6163,7 +6806,7 @@
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>11.16</v>
       </c>
       <c r="C5">
@@ -6698,22 +7341,22 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
@@ -7544,27 +8187,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -8332,4 +8975,673 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="2" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1</v>
+      </c>
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1</v>
+      </c>
+      <c r="I2" s="11">
+        <v>1</v>
+      </c>
+      <c r="J2" s="11">
+        <v>1</v>
+      </c>
+      <c r="K2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8">
+        <v>4</v>
+      </c>
+      <c r="H3" s="8">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1</v>
+      </c>
+      <c r="J3" s="8">
+        <v>16</v>
+      </c>
+      <c r="K3" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15">
+        <v>2</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15">
+        <v>2</v>
+      </c>
+      <c r="F4" s="15">
+        <v>4</v>
+      </c>
+      <c r="G4" s="15">
+        <v>1</v>
+      </c>
+      <c r="H4" s="15">
+        <v>4</v>
+      </c>
+      <c r="I4" s="15">
+        <v>16</v>
+      </c>
+      <c r="J4" s="15">
+        <v>1</v>
+      </c>
+      <c r="K4" s="15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13">
+        <v>13.06</v>
+      </c>
+      <c r="C5">
+        <v>11.14</v>
+      </c>
+      <c r="D5" s="3">
+        <v>11.3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5.78</v>
+      </c>
+      <c r="F5" s="3">
+        <v>6.36</v>
+      </c>
+      <c r="G5" s="3">
+        <v>6.84</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.55</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1.54</v>
+      </c>
+      <c r="J5" s="3">
+        <v>3.15</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="D6" s="2">
+        <v>11.18</v>
+      </c>
+      <c r="E6" s="2">
+        <v>7.01</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
+        <v>7.05</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1.55</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <v>6.19</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1.32</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3">
+        <v>2.02</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3">
+        <v>6.42</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1.56</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3">
+        <v>1.43</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3">
+        <v>1.38</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="1">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="J11" s="3">
+        <v>1.28</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="1">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="J12">
+        <v>2.42</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="1">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3">
+        <v>1.29</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="1">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3">
+        <v>1.63</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="1">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3">
+        <v>1.68</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="1">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3">
+        <v>1.68</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="1">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3">
+        <v>2.13</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="1">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3">
+        <v>2.16</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="1">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3">
+        <v>2.72</v>
+      </c>
+      <c r="K20" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="1">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="1">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="1">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="1">
+        <v>20</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="5">
+        <f t="shared" ref="B25:K25" si="0">AVERAGE(B5:B24)</f>
+        <v>13.06</v>
+      </c>
+      <c r="C25" s="5">
+        <f t="shared" si="0"/>
+        <v>11.14</v>
+      </c>
+      <c r="D25" s="5">
+        <f>AVERAGE(D5:D24)</f>
+        <v>11.24</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="0"/>
+        <v>6.3949999999999996</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="0"/>
+        <v>6.36</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="0"/>
+        <v>6.625</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" si="0"/>
+        <v>1.4950000000000001</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" si="0"/>
+        <v>1.54</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9868749999999995</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="0"/>
+        <v>5.812500000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="5">
+        <f t="shared" ref="B26:K26" si="1">SUM(B5:B24)</f>
+        <v>13.06</v>
+      </c>
+      <c r="C26" s="5">
+        <f t="shared" si="1"/>
+        <v>11.14</v>
+      </c>
+      <c r="D26" s="5">
+        <f>SUM(D5:D24)</f>
+        <v>22.48</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" ref="E26" si="2">SUM(E5:E24)</f>
+        <v>12.79</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="1"/>
+        <v>6.36</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" si="1"/>
+        <v>26.5</v>
+      </c>
+      <c r="H26" s="5">
+        <f t="shared" si="1"/>
+        <v>5.98</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" si="1"/>
+        <v>1.54</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" si="1"/>
+        <v>31.789999999999992</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" si="1"/>
+        <v>0.93000000000000016</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="e">
+        <f t="shared" ref="B27:K27" si="3">STDEVA(B5:B24)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C27" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D27" s="5">
+        <f>STDEVA(D5:D24)</f>
+        <v>8.4852813742386402E-2</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" ref="E27" si="4">STDEVA(E5:E24)</f>
+        <v>0.86974134085945309</v>
+      </c>
+      <c r="F27" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="3"/>
+        <v>0.39076847365159822</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="3"/>
+        <v>0.11676186592091328</v>
+      </c>
+      <c r="I27" s="5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J27" s="5">
+        <f t="shared" si="3"/>
+        <v>0.54498585608558237</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" si="3"/>
+        <v>4.3851073723076207E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <phoneticPr fontId="5"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>